<commit_message>
update for kbv pk
</commit_message>
<xml_diff>
--- a/data/plotdata/sti_ag_bund_plot_data.xlsx
+++ b/data/plotdata/sti_ag_bund_plot_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t xml:space="preserve">JahrKW</t>
   </si>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">STI</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-01</t>
+    <t xml:space="preserve">2020-02</t>
   </si>
   <si>
     <t xml:space="preserve">0-59</t>
@@ -38,9 +38,6 @@
     <t xml:space="preserve">80+</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-02</t>
-  </si>
-  <si>
     <t xml:space="preserve">2020-03</t>
   </si>
   <si>
@@ -195,6 +192,60 @@
   </si>
   <si>
     <t xml:space="preserve">2021-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-19</t>
   </si>
 </sst>
 </file>
@@ -551,7 +602,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43835</v>
+        <v>43842</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -565,7 +616,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43835</v>
+        <v>43842</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -579,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43835</v>
+        <v>43842</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -593,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43842</v>
+        <v>43849</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -607,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43842</v>
+        <v>43849</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -621,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43842</v>
+        <v>43849</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -635,7 +686,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43849</v>
+        <v>43856</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -649,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>43849</v>
+        <v>43856</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -663,7 +714,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>43849</v>
+        <v>43856</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -677,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>43856</v>
+        <v>43863</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -691,7 +742,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>43856</v>
+        <v>43863</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -705,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>43856</v>
+        <v>43863</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -719,7 +770,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>43863</v>
+        <v>43870</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -733,7 +784,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>43863</v>
+        <v>43870</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -747,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>43863</v>
+        <v>43870</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -761,7 +812,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>43870</v>
+        <v>43877</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -775,7 +826,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>43870</v>
+        <v>43877</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -789,7 +840,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>43870</v>
+        <v>43877</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -803,7 +854,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>43877</v>
+        <v>43884</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -817,7 +868,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>43877</v>
+        <v>43884</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -831,7 +882,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>43877</v>
+        <v>43884</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -845,7 +896,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>43884</v>
+        <v>43891</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -859,7 +910,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>43884</v>
+        <v>43891</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -873,7 +924,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>43884</v>
+        <v>43891</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -887,13 +938,13 @@
         <v>15</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>43891</v>
+        <v>43898</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -901,13 +952,13 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>43891</v>
+        <v>43898</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -915,7 +966,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>43891</v>
+        <v>43898</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -929,13 +980,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>43898</v>
+        <v>43905</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -943,13 +994,13 @@
         <v>16</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>43898</v>
+        <v>43905</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -957,13 +1008,13 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>43898</v>
+        <v>43905</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
@@ -971,13 +1022,13 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>43905</v>
+        <v>43912</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
@@ -985,13 +1036,13 @@
         <v>17</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>43905</v>
+        <v>43912</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34">
@@ -999,13 +1050,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>43905</v>
+        <v>43912</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -1013,13 +1064,13 @@
         <v>18</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>43912</v>
+        <v>43919</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36">
@@ -1027,13 +1078,13 @@
         <v>18</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>43912</v>
+        <v>43919</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37">
@@ -1041,13 +1092,13 @@
         <v>18</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>43912</v>
+        <v>43919</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38">
@@ -1055,13 +1106,13 @@
         <v>19</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>43919</v>
+        <v>43926</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39">
@@ -1069,13 +1120,13 @@
         <v>19</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>43919</v>
+        <v>43926</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40">
@@ -1083,13 +1134,13 @@
         <v>19</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>43919</v>
+        <v>43926</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="n">
-        <v>43</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41">
@@ -1097,13 +1148,13 @@
         <v>20</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>43926</v>
+        <v>43933</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42">
@@ -1111,13 +1162,13 @@
         <v>20</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>43926</v>
+        <v>43933</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43">
@@ -1125,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>43926</v>
+        <v>43933</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44">
@@ -1139,13 +1190,13 @@
         <v>21</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>43933</v>
+        <v>43940</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45">
@@ -1153,13 +1204,13 @@
         <v>21</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>43933</v>
+        <v>43940</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46">
@@ -1167,13 +1218,13 @@
         <v>21</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>43933</v>
+        <v>43940</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="n">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47">
@@ -1181,13 +1232,13 @@
         <v>22</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>43940</v>
+        <v>43947</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
       <c r="D47" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -1195,13 +1246,13 @@
         <v>22</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>43940</v>
+        <v>43947</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
@@ -1209,13 +1260,13 @@
         <v>22</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>43940</v>
+        <v>43947</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50">
@@ -1223,13 +1274,13 @@
         <v>23</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>43947</v>
+        <v>43954</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51">
@@ -1237,13 +1288,13 @@
         <v>23</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>43947</v>
+        <v>43954</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1251,13 +1302,13 @@
         <v>23</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>43947</v>
+        <v>43954</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53">
@@ -1265,13 +1316,13 @@
         <v>24</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -1279,13 +1330,13 @@
         <v>24</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -1293,13 +1344,13 @@
         <v>24</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>43954</v>
+        <v>43961</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
       </c>
       <c r="D55" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
@@ -1307,13 +1358,13 @@
         <v>25</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>43961</v>
+        <v>43968</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
       <c r="D56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -1321,13 +1372,13 @@
         <v>25</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>43961</v>
+        <v>43968</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -1335,13 +1386,13 @@
         <v>25</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>43961</v>
+        <v>43968</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
       </c>
       <c r="D58" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59">
@@ -1349,13 +1400,13 @@
         <v>26</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>43968</v>
+        <v>43975</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -1363,13 +1414,13 @@
         <v>26</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>43968</v>
+        <v>43975</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -1377,13 +1428,13 @@
         <v>26</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>43968</v>
+        <v>43975</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
       </c>
       <c r="D61" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -1391,13 +1442,13 @@
         <v>27</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>43975</v>
+        <v>43982</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -1405,13 +1456,13 @@
         <v>27</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>43975</v>
+        <v>43982</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -1419,13 +1470,13 @@
         <v>27</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>43975</v>
+        <v>43982</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
       </c>
       <c r="D64" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -1433,13 +1484,13 @@
         <v>28</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>43982</v>
+        <v>43989</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -1447,7 +1498,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>43982</v>
+        <v>43989</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
@@ -1461,13 +1512,13 @@
         <v>28</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>43982</v>
+        <v>43989</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
       </c>
       <c r="D67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -1475,7 +1526,7 @@
         <v>29</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>43989</v>
+        <v>43996</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -1489,13 +1540,13 @@
         <v>29</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>43989</v>
+        <v>43996</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1503,7 +1554,7 @@
         <v>29</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>43989</v>
+        <v>43996</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -1517,13 +1568,13 @@
         <v>30</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>43996</v>
+        <v>44003</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
       </c>
       <c r="D71" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
@@ -1531,13 +1582,13 @@
         <v>30</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>43996</v>
+        <v>44003</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -1545,7 +1596,7 @@
         <v>30</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>43996</v>
+        <v>44003</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
@@ -1559,13 +1610,13 @@
         <v>31</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>44003</v>
+        <v>44010</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -1573,13 +1624,13 @@
         <v>31</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>44003</v>
+        <v>44010</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -1587,13 +1638,13 @@
         <v>31</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>44003</v>
+        <v>44010</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
       </c>
       <c r="D76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -1601,13 +1652,13 @@
         <v>32</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>44010</v>
+        <v>44017</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
       </c>
       <c r="D77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -1615,7 +1666,7 @@
         <v>32</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>44010</v>
+        <v>44017</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -1629,7 +1680,7 @@
         <v>32</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>44010</v>
+        <v>44017</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -1643,7 +1694,7 @@
         <v>33</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>44017</v>
+        <v>44024</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -1657,7 +1708,7 @@
         <v>33</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>44017</v>
+        <v>44024</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
@@ -1671,13 +1722,13 @@
         <v>33</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>44017</v>
+        <v>44024</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
       </c>
       <c r="D82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -1685,7 +1736,7 @@
         <v>34</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>44024</v>
+        <v>44031</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
@@ -1699,13 +1750,13 @@
         <v>34</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>44024</v>
+        <v>44031</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -1713,13 +1764,13 @@
         <v>34</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>44024</v>
+        <v>44031</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
@@ -1727,13 +1778,13 @@
         <v>35</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>44031</v>
+        <v>44038</v>
       </c>
       <c r="C86" t="s">
         <v>5</v>
       </c>
       <c r="D86" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87">
@@ -1741,7 +1792,7 @@
         <v>35</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>44031</v>
+        <v>44038</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
@@ -1755,7 +1806,7 @@
         <v>35</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>44031</v>
+        <v>44038</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
@@ -1769,13 +1820,13 @@
         <v>36</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>44038</v>
+        <v>44045</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
       </c>
       <c r="D89" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
@@ -1783,7 +1834,7 @@
         <v>36</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>44038</v>
+        <v>44045</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
@@ -1797,13 +1848,13 @@
         <v>36</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>44038</v>
+        <v>44045</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92">
@@ -1811,13 +1862,13 @@
         <v>37</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
       </c>
       <c r="D92" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93">
@@ -1825,13 +1876,13 @@
         <v>37</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -1839,13 +1890,13 @@
         <v>37</v>
       </c>
       <c r="B94" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="C94" t="s">
         <v>7</v>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95">
@@ -1853,13 +1904,13 @@
         <v>38</v>
       </c>
       <c r="B95" s="1" t="n">
-        <v>44052</v>
+        <v>44059</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
       </c>
       <c r="D95" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96">
@@ -1867,7 +1918,7 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="n">
-        <v>44052</v>
+        <v>44059</v>
       </c>
       <c r="C96" t="s">
         <v>6</v>
@@ -1881,13 +1932,13 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="n">
-        <v>44052</v>
+        <v>44059</v>
       </c>
       <c r="C97" t="s">
         <v>7</v>
       </c>
       <c r="D97" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -1895,13 +1946,13 @@
         <v>39</v>
       </c>
       <c r="B98" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
       <c r="D98" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99">
@@ -1909,7 +1960,7 @@
         <v>39</v>
       </c>
       <c r="B99" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="C99" t="s">
         <v>6</v>
@@ -1923,13 +1974,13 @@
         <v>39</v>
       </c>
       <c r="B100" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
       </c>
       <c r="D100" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -1937,13 +1988,13 @@
         <v>40</v>
       </c>
       <c r="B101" s="1" t="n">
-        <v>44066</v>
+        <v>44073</v>
       </c>
       <c r="C101" t="s">
         <v>5</v>
       </c>
       <c r="D101" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102">
@@ -1951,7 +2002,7 @@
         <v>40</v>
       </c>
       <c r="B102" s="1" t="n">
-        <v>44066</v>
+        <v>44073</v>
       </c>
       <c r="C102" t="s">
         <v>6</v>
@@ -1965,7 +2016,7 @@
         <v>40</v>
       </c>
       <c r="B103" s="1" t="n">
-        <v>44066</v>
+        <v>44073</v>
       </c>
       <c r="C103" t="s">
         <v>7</v>
@@ -1979,13 +2030,13 @@
         <v>41</v>
       </c>
       <c r="B104" s="1" t="n">
-        <v>44073</v>
+        <v>44080</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
       </c>
       <c r="D104" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105">
@@ -1993,7 +2044,7 @@
         <v>41</v>
       </c>
       <c r="B105" s="1" t="n">
-        <v>44073</v>
+        <v>44080</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
@@ -2007,7 +2058,7 @@
         <v>41</v>
       </c>
       <c r="B106" s="1" t="n">
-        <v>44073</v>
+        <v>44080</v>
       </c>
       <c r="C106" t="s">
         <v>7</v>
@@ -2021,13 +2072,13 @@
         <v>42</v>
       </c>
       <c r="B107" s="1" t="n">
-        <v>44080</v>
+        <v>44087</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
       </c>
       <c r="D107" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108">
@@ -2035,13 +2086,13 @@
         <v>42</v>
       </c>
       <c r="B108" s="1" t="n">
-        <v>44080</v>
+        <v>44087</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109">
@@ -2049,13 +2100,13 @@
         <v>42</v>
       </c>
       <c r="B109" s="1" t="n">
-        <v>44080</v>
+        <v>44087</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
       </c>
       <c r="D109" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -2063,13 +2114,13 @@
         <v>43</v>
       </c>
       <c r="B110" s="1" t="n">
-        <v>44087</v>
+        <v>44094</v>
       </c>
       <c r="C110" t="s">
         <v>5</v>
       </c>
       <c r="D110" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="111">
@@ -2077,13 +2128,13 @@
         <v>43</v>
       </c>
       <c r="B111" s="1" t="n">
-        <v>44087</v>
+        <v>44094</v>
       </c>
       <c r="C111" t="s">
         <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
@@ -2091,13 +2142,13 @@
         <v>43</v>
       </c>
       <c r="B112" s="1" t="n">
-        <v>44087</v>
+        <v>44094</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
@@ -2105,13 +2156,13 @@
         <v>44</v>
       </c>
       <c r="B113" s="1" t="n">
-        <v>44094</v>
+        <v>44101</v>
       </c>
       <c r="C113" t="s">
         <v>5</v>
       </c>
       <c r="D113" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="114">
@@ -2119,7 +2170,7 @@
         <v>44</v>
       </c>
       <c r="B114" s="1" t="n">
-        <v>44094</v>
+        <v>44101</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
@@ -2133,13 +2184,13 @@
         <v>44</v>
       </c>
       <c r="B115" s="1" t="n">
-        <v>44094</v>
+        <v>44101</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
       </c>
       <c r="D115" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116">
@@ -2147,13 +2198,13 @@
         <v>45</v>
       </c>
       <c r="B116" s="1" t="n">
-        <v>44101</v>
+        <v>44108</v>
       </c>
       <c r="C116" t="s">
         <v>5</v>
       </c>
       <c r="D116" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117">
@@ -2161,13 +2212,13 @@
         <v>45</v>
       </c>
       <c r="B117" s="1" t="n">
-        <v>44101</v>
+        <v>44108</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118">
@@ -2175,13 +2226,13 @@
         <v>45</v>
       </c>
       <c r="B118" s="1" t="n">
-        <v>44101</v>
+        <v>44108</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
       </c>
       <c r="D118" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119">
@@ -2189,13 +2240,13 @@
         <v>46</v>
       </c>
       <c r="B119" s="1" t="n">
-        <v>44108</v>
+        <v>44115</v>
       </c>
       <c r="C119" t="s">
         <v>5</v>
       </c>
       <c r="D119" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="120">
@@ -2203,13 +2254,13 @@
         <v>46</v>
       </c>
       <c r="B120" s="1" t="n">
-        <v>44108</v>
+        <v>44115</v>
       </c>
       <c r="C120" t="s">
         <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121">
@@ -2217,13 +2268,13 @@
         <v>46</v>
       </c>
       <c r="B121" s="1" t="n">
-        <v>44108</v>
+        <v>44115</v>
       </c>
       <c r="C121" t="s">
         <v>7</v>
       </c>
       <c r="D121" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122">
@@ -2231,13 +2282,13 @@
         <v>47</v>
       </c>
       <c r="B122" s="1" t="n">
-        <v>44115</v>
+        <v>44122</v>
       </c>
       <c r="C122" t="s">
         <v>5</v>
       </c>
       <c r="D122" t="n">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="123">
@@ -2245,13 +2296,13 @@
         <v>47</v>
       </c>
       <c r="B123" s="1" t="n">
-        <v>44115</v>
+        <v>44122</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
       </c>
       <c r="D123" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124">
@@ -2259,13 +2310,13 @@
         <v>47</v>
       </c>
       <c r="B124" s="1" t="n">
-        <v>44115</v>
+        <v>44122</v>
       </c>
       <c r="C124" t="s">
         <v>7</v>
       </c>
       <c r="D124" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125">
@@ -2273,13 +2324,13 @@
         <v>48</v>
       </c>
       <c r="B125" s="1" t="n">
-        <v>44122</v>
+        <v>44129</v>
       </c>
       <c r="C125" t="s">
         <v>5</v>
       </c>
       <c r="D125" t="n">
-        <v>59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="126">
@@ -2287,13 +2338,13 @@
         <v>48</v>
       </c>
       <c r="B126" s="1" t="n">
-        <v>44122</v>
+        <v>44129</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="n">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="127">
@@ -2301,13 +2352,13 @@
         <v>48</v>
       </c>
       <c r="B127" s="1" t="n">
-        <v>44122</v>
+        <v>44129</v>
       </c>
       <c r="C127" t="s">
         <v>7</v>
       </c>
       <c r="D127" t="n">
-        <v>33</v>
+        <v>68</v>
       </c>
     </row>
     <row r="128">
@@ -2315,13 +2366,13 @@
         <v>49</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>44129</v>
+        <v>44136</v>
       </c>
       <c r="C128" t="s">
         <v>5</v>
       </c>
       <c r="D128" t="n">
-        <v>103</v>
+        <v>151</v>
       </c>
     </row>
     <row r="129">
@@ -2329,13 +2380,13 @@
         <v>49</v>
       </c>
       <c r="B129" s="1" t="n">
-        <v>44129</v>
+        <v>44136</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="n">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="130">
@@ -2343,13 +2394,13 @@
         <v>49</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>44129</v>
+        <v>44136</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
       </c>
       <c r="D130" t="n">
-        <v>68</v>
+        <v>107</v>
       </c>
     </row>
     <row r="131">
@@ -2357,13 +2408,13 @@
         <v>50</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
       </c>
       <c r="D131" t="n">
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="132">
@@ -2371,13 +2422,13 @@
         <v>50</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="C132" t="s">
         <v>6</v>
       </c>
       <c r="D132" t="n">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="133">
@@ -2385,13 +2436,13 @@
         <v>50</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
       </c>
       <c r="D133" t="n">
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="134">
@@ -2399,13 +2450,13 @@
         <v>51</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>44143</v>
+        <v>44150</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
       </c>
       <c r="D134" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135">
@@ -2413,13 +2464,13 @@
         <v>51</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>44143</v>
+        <v>44150</v>
       </c>
       <c r="C135" t="s">
         <v>6</v>
       </c>
       <c r="D135" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="136">
@@ -2427,13 +2478,13 @@
         <v>51</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>44143</v>
+        <v>44150</v>
       </c>
       <c r="C136" t="s">
         <v>7</v>
       </c>
       <c r="D136" t="n">
-        <v>131</v>
+        <v>158</v>
       </c>
     </row>
     <row r="137">
@@ -2441,13 +2492,13 @@
         <v>52</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>44150</v>
+        <v>44157</v>
       </c>
       <c r="C137" t="s">
         <v>5</v>
       </c>
       <c r="D137" t="n">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="138">
@@ -2455,13 +2506,13 @@
         <v>52</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>44150</v>
+        <v>44157</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
       </c>
       <c r="D138" t="n">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="139">
@@ -2469,13 +2520,13 @@
         <v>52</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>44150</v>
+        <v>44157</v>
       </c>
       <c r="C139" t="s">
         <v>7</v>
       </c>
       <c r="D139" t="n">
-        <v>157</v>
+        <v>190</v>
       </c>
     </row>
     <row r="140">
@@ -2483,13 +2534,13 @@
         <v>53</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>44157</v>
+        <v>44164</v>
       </c>
       <c r="C140" t="s">
         <v>5</v>
       </c>
       <c r="D140" t="n">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="141">
@@ -2497,13 +2548,13 @@
         <v>53</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>44157</v>
+        <v>44164</v>
       </c>
       <c r="C141" t="s">
         <v>6</v>
       </c>
       <c r="D141" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="142">
@@ -2511,13 +2562,13 @@
         <v>53</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>44157</v>
+        <v>44164</v>
       </c>
       <c r="C142" t="s">
         <v>7</v>
       </c>
       <c r="D142" t="n">
-        <v>190</v>
+        <v>218</v>
       </c>
     </row>
     <row r="143">
@@ -2525,13 +2576,13 @@
         <v>54</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>44164</v>
+        <v>44171</v>
       </c>
       <c r="C143" t="s">
         <v>5</v>
       </c>
       <c r="D143" t="n">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="144">
@@ -2539,13 +2590,13 @@
         <v>54</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>44164</v>
+        <v>44171</v>
       </c>
       <c r="C144" t="s">
         <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="145">
@@ -2553,13 +2604,13 @@
         <v>54</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>44164</v>
+        <v>44171</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
       </c>
       <c r="D145" t="n">
-        <v>218</v>
+        <v>250</v>
       </c>
     </row>
     <row r="146">
@@ -2567,13 +2618,13 @@
         <v>55</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>44171</v>
+        <v>44178</v>
       </c>
       <c r="C146" t="s">
         <v>5</v>
       </c>
       <c r="D146" t="n">
-        <v>159</v>
+        <v>192</v>
       </c>
     </row>
     <row r="147">
@@ -2581,13 +2632,13 @@
         <v>55</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>44171</v>
+        <v>44178</v>
       </c>
       <c r="C147" t="s">
         <v>6</v>
       </c>
       <c r="D147" t="n">
-        <v>106</v>
+        <v>133</v>
       </c>
     </row>
     <row r="148">
@@ -2595,13 +2646,13 @@
         <v>55</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>44171</v>
+        <v>44178</v>
       </c>
       <c r="C148" t="s">
         <v>7</v>
       </c>
       <c r="D148" t="n">
-        <v>249</v>
+        <v>324</v>
       </c>
     </row>
     <row r="149">
@@ -2609,13 +2660,13 @@
         <v>56</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>44178</v>
+        <v>44185</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
       </c>
       <c r="D149" t="n">
-        <v>191</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150">
@@ -2623,13 +2674,13 @@
         <v>56</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>44178</v>
+        <v>44185</v>
       </c>
       <c r="C150" t="s">
         <v>6</v>
       </c>
       <c r="D150" t="n">
-        <v>132</v>
+        <v>158</v>
       </c>
     </row>
     <row r="151">
@@ -2637,13 +2688,13 @@
         <v>56</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>44178</v>
+        <v>44185</v>
       </c>
       <c r="C151" t="s">
         <v>7</v>
       </c>
       <c r="D151" t="n">
-        <v>323</v>
+        <v>373</v>
       </c>
     </row>
     <row r="152">
@@ -2651,13 +2702,13 @@
         <v>57</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>44185</v>
+        <v>44192</v>
       </c>
       <c r="C152" t="s">
         <v>5</v>
       </c>
       <c r="D152" t="n">
-        <v>209</v>
+        <v>162</v>
       </c>
     </row>
     <row r="153">
@@ -2665,13 +2716,13 @@
         <v>57</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>44185</v>
+        <v>44192</v>
       </c>
       <c r="C153" t="s">
         <v>6</v>
       </c>
       <c r="D153" t="n">
-        <v>157</v>
+        <v>135</v>
       </c>
     </row>
     <row r="154">
@@ -2679,13 +2730,13 @@
         <v>57</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>44185</v>
+        <v>44192</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
       </c>
       <c r="D154" t="n">
-        <v>371</v>
+        <v>326</v>
       </c>
     </row>
     <row r="155">
@@ -2693,13 +2744,13 @@
         <v>58</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>44192</v>
+        <v>44199</v>
       </c>
       <c r="C155" t="s">
         <v>5</v>
       </c>
       <c r="D155" t="n">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="156">
@@ -2707,13 +2758,13 @@
         <v>58</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>44192</v>
+        <v>44199</v>
       </c>
       <c r="C156" t="s">
         <v>6</v>
       </c>
       <c r="D156" t="n">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="157">
@@ -2721,13 +2772,13 @@
         <v>58</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>44192</v>
+        <v>44199</v>
       </c>
       <c r="C157" t="s">
         <v>7</v>
       </c>
       <c r="D157" t="n">
-        <v>325</v>
+        <v>307</v>
       </c>
     </row>
     <row r="158">
@@ -2735,13 +2786,13 @@
         <v>59</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>44199</v>
+        <v>44206</v>
       </c>
       <c r="C158" t="s">
         <v>5</v>
       </c>
       <c r="D158" t="n">
-        <v>140</v>
+        <v>170</v>
       </c>
     </row>
     <row r="159">
@@ -2749,13 +2800,13 @@
         <v>59</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>44199</v>
+        <v>44206</v>
       </c>
       <c r="C159" t="s">
         <v>6</v>
       </c>
       <c r="D159" t="n">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="160">
@@ -2763,13 +2814,13 @@
         <v>59</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>44199</v>
+        <v>44206</v>
       </c>
       <c r="C160" t="s">
         <v>7</v>
       </c>
       <c r="D160" t="n">
-        <v>305</v>
+        <v>337</v>
       </c>
     </row>
     <row r="161">
@@ -2777,13 +2828,13 @@
         <v>60</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>44206</v>
+        <v>44213</v>
       </c>
       <c r="C161" t="s">
         <v>5</v>
       </c>
       <c r="D161" t="n">
-        <v>167</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162">
@@ -2791,13 +2842,13 @@
         <v>60</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>44206</v>
+        <v>44213</v>
       </c>
       <c r="C162" t="s">
         <v>6</v>
       </c>
       <c r="D162" t="n">
-        <v>136</v>
+        <v>111</v>
       </c>
     </row>
     <row r="163">
@@ -2805,13 +2856,727 @@
         <v>60</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>44206</v>
+        <v>44213</v>
       </c>
       <c r="C163" t="s">
         <v>7</v>
       </c>
       <c r="D163" t="n">
-        <v>331</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>61</v>
+      </c>
+      <c r="B164" s="1" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C164" t="s">
+        <v>5</v>
+      </c>
+      <c r="D164" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>61</v>
+      </c>
+      <c r="B165" s="1" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C165" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>61</v>
+      </c>
+      <c r="B166" s="1" t="n">
+        <v>44220</v>
+      </c>
+      <c r="C166" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>62</v>
+      </c>
+      <c r="B167" s="1" t="n">
+        <v>44227</v>
+      </c>
+      <c r="C167" t="s">
+        <v>5</v>
+      </c>
+      <c r="D167" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>62</v>
+      </c>
+      <c r="B168" s="1" t="n">
+        <v>44227</v>
+      </c>
+      <c r="C168" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>62</v>
+      </c>
+      <c r="B169" s="1" t="n">
+        <v>44227</v>
+      </c>
+      <c r="C169" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" t="n">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>63</v>
+      </c>
+      <c r="B170" s="1" t="n">
+        <v>44234</v>
+      </c>
+      <c r="C170" t="s">
+        <v>5</v>
+      </c>
+      <c r="D170" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>63</v>
+      </c>
+      <c r="B171" s="1" t="n">
+        <v>44234</v>
+      </c>
+      <c r="C171" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>63</v>
+      </c>
+      <c r="B172" s="1" t="n">
+        <v>44234</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>64</v>
+      </c>
+      <c r="B173" s="1" t="n">
+        <v>44241</v>
+      </c>
+      <c r="C173" t="s">
+        <v>5</v>
+      </c>
+      <c r="D173" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>64</v>
+      </c>
+      <c r="B174" s="1" t="n">
+        <v>44241</v>
+      </c>
+      <c r="C174" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>64</v>
+      </c>
+      <c r="B175" s="1" t="n">
+        <v>44241</v>
+      </c>
+      <c r="C175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>65</v>
+      </c>
+      <c r="B176" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="C176" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>65</v>
+      </c>
+      <c r="B177" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="C177" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>65</v>
+      </c>
+      <c r="B178" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="C178" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>66</v>
+      </c>
+      <c r="B179" s="1" t="n">
+        <v>44255</v>
+      </c>
+      <c r="C179" t="s">
+        <v>5</v>
+      </c>
+      <c r="D179" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>66</v>
+      </c>
+      <c r="B180" s="1" t="n">
+        <v>44255</v>
+      </c>
+      <c r="C180" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>66</v>
+      </c>
+      <c r="B181" s="1" t="n">
+        <v>44255</v>
+      </c>
+      <c r="C181" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>67</v>
+      </c>
+      <c r="B182" s="1" t="n">
+        <v>44262</v>
+      </c>
+      <c r="C182" t="s">
+        <v>5</v>
+      </c>
+      <c r="D182" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>67</v>
+      </c>
+      <c r="B183" s="1" t="n">
+        <v>44262</v>
+      </c>
+      <c r="C183" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>67</v>
+      </c>
+      <c r="B184" s="1" t="n">
+        <v>44262</v>
+      </c>
+      <c r="C184" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>68</v>
+      </c>
+      <c r="B185" s="1" t="n">
+        <v>44269</v>
+      </c>
+      <c r="C185" t="s">
+        <v>5</v>
+      </c>
+      <c r="D185" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>68</v>
+      </c>
+      <c r="B186" s="1" t="n">
+        <v>44269</v>
+      </c>
+      <c r="C186" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>68</v>
+      </c>
+      <c r="B187" s="1" t="n">
+        <v>44269</v>
+      </c>
+      <c r="C187" t="s">
+        <v>7</v>
+      </c>
+      <c r="D187" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>69</v>
+      </c>
+      <c r="B188" s="1" t="n">
+        <v>44276</v>
+      </c>
+      <c r="C188" t="s">
+        <v>5</v>
+      </c>
+      <c r="D188" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>69</v>
+      </c>
+      <c r="B189" s="1" t="n">
+        <v>44276</v>
+      </c>
+      <c r="C189" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>69</v>
+      </c>
+      <c r="B190" s="1" t="n">
+        <v>44276</v>
+      </c>
+      <c r="C190" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>70</v>
+      </c>
+      <c r="B191" s="1" t="n">
+        <v>44283</v>
+      </c>
+      <c r="C191" t="s">
+        <v>5</v>
+      </c>
+      <c r="D191" t="n">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>70</v>
+      </c>
+      <c r="B192" s="1" t="n">
+        <v>44283</v>
+      </c>
+      <c r="C192" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>70</v>
+      </c>
+      <c r="B193" s="1" t="n">
+        <v>44283</v>
+      </c>
+      <c r="C193" t="s">
+        <v>7</v>
+      </c>
+      <c r="D193" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>71</v>
+      </c>
+      <c r="B194" s="1" t="n">
+        <v>44290</v>
+      </c>
+      <c r="C194" t="s">
+        <v>5</v>
+      </c>
+      <c r="D194" t="n">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>71</v>
+      </c>
+      <c r="B195" s="1" t="n">
+        <v>44290</v>
+      </c>
+      <c r="C195" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>71</v>
+      </c>
+      <c r="B196" s="1" t="n">
+        <v>44290</v>
+      </c>
+      <c r="C196" t="s">
+        <v>7</v>
+      </c>
+      <c r="D196" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>72</v>
+      </c>
+      <c r="B197" s="1" t="n">
+        <v>44297</v>
+      </c>
+      <c r="C197" t="s">
+        <v>5</v>
+      </c>
+      <c r="D197" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>72</v>
+      </c>
+      <c r="B198" s="1" t="n">
+        <v>44297</v>
+      </c>
+      <c r="C198" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>72</v>
+      </c>
+      <c r="B199" s="1" t="n">
+        <v>44297</v>
+      </c>
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>73</v>
+      </c>
+      <c r="B200" s="1" t="n">
+        <v>44304</v>
+      </c>
+      <c r="C200" t="s">
+        <v>5</v>
+      </c>
+      <c r="D200" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>73</v>
+      </c>
+      <c r="B201" s="1" t="n">
+        <v>44304</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>73</v>
+      </c>
+      <c r="B202" s="1" t="n">
+        <v>44304</v>
+      </c>
+      <c r="C202" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>74</v>
+      </c>
+      <c r="B203" s="1" t="n">
+        <v>44311</v>
+      </c>
+      <c r="C203" t="s">
+        <v>5</v>
+      </c>
+      <c r="D203" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>74</v>
+      </c>
+      <c r="B204" s="1" t="n">
+        <v>44311</v>
+      </c>
+      <c r="C204" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>74</v>
+      </c>
+      <c r="B205" s="1" t="n">
+        <v>44311</v>
+      </c>
+      <c r="C205" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>75</v>
+      </c>
+      <c r="B206" s="1" t="n">
+        <v>44318</v>
+      </c>
+      <c r="C206" t="s">
+        <v>5</v>
+      </c>
+      <c r="D206" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>75</v>
+      </c>
+      <c r="B207" s="1" t="n">
+        <v>44318</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>75</v>
+      </c>
+      <c r="B208" s="1" t="n">
+        <v>44318</v>
+      </c>
+      <c r="C208" t="s">
+        <v>7</v>
+      </c>
+      <c r="D208" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>76</v>
+      </c>
+      <c r="B209" s="1" t="n">
+        <v>44325</v>
+      </c>
+      <c r="C209" t="s">
+        <v>5</v>
+      </c>
+      <c r="D209" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>76</v>
+      </c>
+      <c r="B210" s="1" t="n">
+        <v>44325</v>
+      </c>
+      <c r="C210" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>76</v>
+      </c>
+      <c r="B211" s="1" t="n">
+        <v>44325</v>
+      </c>
+      <c r="C211" t="s">
+        <v>7</v>
+      </c>
+      <c r="D211" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>77</v>
+      </c>
+      <c r="B212" s="1" t="n">
+        <v>44332</v>
+      </c>
+      <c r="C212" t="s">
+        <v>5</v>
+      </c>
+      <c r="D212" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>77</v>
+      </c>
+      <c r="B213" s="1" t="n">
+        <v>44332</v>
+      </c>
+      <c r="C213" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>77</v>
+      </c>
+      <c r="B214" s="1" t="n">
+        <v>44332</v>
+      </c>
+      <c r="C214" t="s">
+        <v>7</v>
+      </c>
+      <c r="D214" t="n">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>